<commit_message>
Add a bit nicer graphs and some extra paragraphs.
</commit_message>
<xml_diff>
--- a/paper/images/results/TimesXMemory1_2BAM.xlsx
+++ b/paper/images/results/TimesXMemory1_2BAM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t xml:space="preserve">Algo</t>
   </si>
@@ -62,12 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">Time Par</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scaling Compact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scaling Par</t>
   </si>
   <si>
     <t xml:space="preserve">BAM_144MB</t>
@@ -202,7 +196,7 @@
       <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFFF38"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -215,7 +209,7 @@
       <rgbColor rgb="FF83CAFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFD7D7"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF81D41A"/>
@@ -237,7 +231,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -369,11 +363,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="70561477"/>
-        <c:axId val="22413224"/>
+        <c:axId val="74026268"/>
+        <c:axId val="82518994"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70561477"/>
+        <c:axId val="74026268"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -429,14 +423,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22413224"/>
+        <c:crossAx val="82518994"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22413224"/>
+        <c:axId val="82518994"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -473,7 +467,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70561477"/>
+        <c:crossAx val="74026268"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -520,7 +514,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -696,12 +690,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="15597740"/>
-        <c:axId val="20229242"/>
+        <c:axId val="38486519"/>
+        <c:axId val="58593058"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="15597740"/>
+        <c:axId val="38486519"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -757,14 +751,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20229242"/>
+        <c:crossAx val="58593058"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20229242"/>
+        <c:axId val="58593058"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -801,7 +795,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15597740"/>
+        <c:crossAx val="38486519"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -819,7 +813,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -987,12 +981,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="14640068"/>
-        <c:axId val="56388991"/>
+        <c:axId val="21675220"/>
+        <c:axId val="61872756"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="14640068"/>
+        <c:axId val="21675220"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1048,14 +1042,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56388991"/>
+        <c:crossAx val="61872756"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56388991"/>
+        <c:axId val="61872756"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1120,7 +1114,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14640068"/>
+        <c:crossAx val="21675220"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1138,7 +1132,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1300,12 +1294,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="22370343"/>
-        <c:axId val="12066544"/>
+        <c:axId val="23500104"/>
+        <c:axId val="89960950"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="22370343"/>
+        <c:axId val="23500104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1333,14 +1327,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12066544"/>
+        <c:crossAx val="89960950"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="12066544"/>
+        <c:axId val="89960950"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1377,7 +1371,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22370343"/>
+        <c:crossAx val="23500104"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1416,11 +1410,40 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>GB / second</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:view3D>
       <c:rotX val="11"/>
       <c:rotY val="25"/>
@@ -1471,15 +1494,23 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Scaling Compact</c:v>
+                  <c:v>Compact</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="7e0021"/>
-            </a:solidFill>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:srgbClr val="ffff38"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:srgbClr val="ffd7d7"/>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="3600000"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1498,7 +1529,7 @@
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
+            <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
@@ -1529,13 +1560,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.197941176470588</c:v>
+                  <c:v>197.94</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.164705882352941</c:v>
+                  <c:v>164.71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.185</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1550,7 +1581,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Scaling Par</c:v>
+                  <c:v>Compact Par</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1577,7 +1608,7 @@
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
+            <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
@@ -1608,13 +1639,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.143803418803419</c:v>
+                  <c:v>143.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.209737827715356</c:v>
+                  <c:v>209.74</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.197709923664122</c:v>
+                  <c:v>197.71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1622,12 +1653,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="51476656"/>
-        <c:axId val="58867308"/>
+        <c:axId val="17609089"/>
+        <c:axId val="74945432"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="51476656"/>
+        <c:axId val="17609089"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1655,14 +1686,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58867308"/>
+        <c:crossAx val="74945432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58867308"/>
+        <c:axId val="74945432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1699,7 +1730,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51476656"/>
+        <c:crossAx val="17609089"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1900,8 +1931,8 @@
   </sheetPr>
   <dimension ref="A3:G75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K72" activeCellId="0" sqref="K72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M79" activeCellId="0" sqref="M79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2162,11 +2193,6 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>9</v>
@@ -2184,15 +2210,15 @@
         <v>13</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>0.144</v>
@@ -2207,17 +2233,17 @@
         <v>4.68</v>
       </c>
       <c r="F73" s="0" t="n">
-        <f aca="false">C73/D73</f>
-        <v>0.197941176470588</v>
+        <f aca="false">ROUND(C73/D73*1000,2)</f>
+        <v>197.94</v>
       </c>
       <c r="G73" s="0" t="n">
-        <f aca="false">C73/E73</f>
-        <v>0.143803418803419</v>
+        <f aca="false">ROUND(C73/E73*1000,2)</f>
+        <v>143.8</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>1.2</v>
@@ -2232,17 +2258,17 @@
         <v>26.7</v>
       </c>
       <c r="F74" s="0" t="n">
-        <f aca="false">C74/D74</f>
-        <v>0.164705882352941</v>
+        <f aca="false">ROUND(C74/D74*1000,2)</f>
+        <v>164.71</v>
       </c>
       <c r="G74" s="0" t="n">
-        <f aca="false">C74/E74</f>
-        <v>0.209737827715356</v>
+        <f aca="false">ROUND(C74/E74*1000,2)</f>
+        <v>209.74</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>8</v>
@@ -2257,12 +2283,12 @@
         <v>131</v>
       </c>
       <c r="F75" s="0" t="n">
-        <f aca="false">C75/D75</f>
-        <v>0.185</v>
+        <f aca="false">ROUND(C75/D75*1000,2)</f>
+        <v>185</v>
       </c>
       <c r="G75" s="0" t="n">
-        <f aca="false">C75/E75</f>
-        <v>0.197709923664122</v>
+        <f aca="false">ROUND(C75/E75*1000,2)</f>
+        <v>197.71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated results. The times are a bit worse because of the "writing bug" but are more correct. Still, it doesn't change values but on laptop/4c.
</commit_message>
<xml_diff>
--- a/paper/images/results/TimesXMemory1_2BAM.xlsx
+++ b/paper/images/results/TimesXMemory1_2BAM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
   <si>
     <t xml:space="preserve">Algo</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Compact Par</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4c</t>
   </si>
   <si>
     <t xml:space="preserve">File Name</t>
@@ -80,11 +83,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -100,6 +104,17 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="DejaVu Sans Mono"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="13"/>
@@ -154,19 +169,27 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -186,7 +209,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FFA9B7C6"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -206,16 +229,16 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF83CAFF"/>
+      <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFD7D7"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF83CAFF"/>
       <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FFBF819E"/>
       <rgbColor rgb="FF003366"/>
@@ -231,7 +254,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -294,23 +317,13 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -363,11 +376,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="74026268"/>
-        <c:axId val="82518994"/>
+        <c:axId val="39982156"/>
+        <c:axId val="62623546"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74026268"/>
+        <c:axId val="39982156"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -423,14 +436,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82518994"/>
+        <c:crossAx val="62623546"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82518994"/>
+        <c:axId val="62623546"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -445,7 +458,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -467,7 +480,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74026268"/>
+        <c:crossAx val="39982156"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -514,7 +527,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -621,23 +634,12 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -690,12 +692,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="38486519"/>
-        <c:axId val="58593058"/>
+        <c:axId val="34199797"/>
+        <c:axId val="77589560"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="38486519"/>
+        <c:axId val="34199797"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,14 +753,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58593058"/>
+        <c:crossAx val="77589560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58593058"/>
+        <c:axId val="77589560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -773,7 +775,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -795,7 +797,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38486519"/>
+        <c:crossAx val="34199797"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -813,7 +815,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -912,23 +914,12 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -981,12 +972,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="21675220"/>
-        <c:axId val="61872756"/>
+        <c:axId val="52000376"/>
+        <c:axId val="51539058"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="21675220"/>
+        <c:axId val="52000376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1042,14 +1033,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61872756"/>
+        <c:crossAx val="51539058"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61872756"/>
+        <c:axId val="51539058"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1092,7 +1083,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1114,7 +1105,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21675220"/>
+        <c:crossAx val="52000376"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1132,7 +1123,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1152,7 +1143,7 @@
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Times x Memory (144 MB BAM File)</a:t>
+              <a:t>Times x Memory 4c (144 MB BAM File)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1231,23 +1222,12 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -1286,7 +1266,7 @@
                   <c:v>20.02</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.91</c:v>
+                  <c:v>3.42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1294,12 +1274,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="23500104"/>
-        <c:axId val="89960950"/>
+        <c:axId val="55761015"/>
+        <c:axId val="85189144"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="23500104"/>
+        <c:axId val="55761015"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1327,14 +1307,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89960950"/>
+        <c:crossAx val="85189144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89960950"/>
+        <c:axId val="85189144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1349,7 +1329,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1371,7 +1351,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23500104"/>
+        <c:crossAx val="55761015"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1410,7 +1390,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1430,7 +1410,7 @@
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>GB / second</a:t>
+              <a:t>MB / second</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1517,23 +1497,12 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -1596,23 +1565,12 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -1653,12 +1611,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="17609089"/>
-        <c:axId val="74945432"/>
+        <c:axId val="57060530"/>
+        <c:axId val="91804926"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="17609089"/>
+        <c:axId val="57060530"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1686,14 +1644,321 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74945432"/>
+        <c:crossAx val="91804926"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74945432"/>
+        <c:axId val="91804926"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="57060530"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>MB / second (4core)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="11"/>
+      <c:rotY val="25"/>
+      <c:rAngAx val="1"/>
+      <c:perspective val="40"/>
+    </c:view3D>
+    <c:floor>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="cccccc"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$78</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Compact</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7e0021"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$79:$F$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>197.94</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$78</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Compact Par</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$79:$G$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>143.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>111.68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:shape val="box"/>
+        <c:axId val="53961887"/>
+        <c:axId val="63720312"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="53961887"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="63720312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="63720312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1730,7 +1995,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17609089"/>
+        <c:crossAx val="53961887"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1780,9 +2045,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>691200</xdr:colOff>
+      <xdr:colOff>690840</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1791,7 +2056,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="386280" y="1816920"/>
-        <a:ext cx="5763240" cy="3241440"/>
+        <a:ext cx="5765400" cy="3241080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1803,16 +2068,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>383040</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>434520</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>456840</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>507960</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>66960</xdr:rowOff>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1820,8 +2085,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6654240" y="726840"/>
-        <a:ext cx="5763240" cy="3241440"/>
+        <a:off x="9151560" y="736560"/>
+        <a:ext cx="5771880" cy="3241080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1840,9 +2105,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>695160</xdr:colOff>
+      <xdr:colOff>694800</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1850,8 +2115,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6080040" y="4475160"/>
-        <a:ext cx="5762880" cy="3241800"/>
+        <a:off x="6082560" y="4475160"/>
+        <a:ext cx="5771520" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1863,16 +2128,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>498240</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>656280</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>73800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>568440</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>726120</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1880,8 +2145,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5956560" y="7714080"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="6931080" y="7714080"/>
+        <a:ext cx="5768280" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1893,16 +2158,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>376920</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>28440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>306360</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>438840</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1910,12 +2175,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5702400" y="12402360"/>
-        <a:ext cx="5751720" cy="3241800"/>
+        <a:off x="11536200" y="10269720"/>
+        <a:ext cx="5760360" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>601920</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>74520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>663120</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>63000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="5248800" y="13892040"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1929,16 +2224,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:G75"/>
+  <dimension ref="A3:G80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M79" activeCellId="0" sqref="M79"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N49" activeCellId="0" sqref="N49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2119,6 +2416,11 @@
         <v>2.88</v>
       </c>
     </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>0</v>
@@ -2182,32 +2484,47 @@
       <c r="A52" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="0" t="n">
-        <v>3.16</v>
+      <c r="B52" s="1" t="n">
+        <v>5.6374</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>0.606</v>
       </c>
       <c r="D52" s="0" t="n">
         <f aca="false">ROUND(B52*C52, 2)</f>
-        <v>1.91</v>
+        <v>3.42</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" s="1" t="n">
+        <v>5.4213</v>
+      </c>
+      <c r="C53" s="2" t="n">
+        <v>0.606</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <f aca="false">ROUND(B53*C53, 2)</f>
+        <v>3.29</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F72" s="0" t="s">
         <v>7</v>
@@ -2218,7 +2535,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>0.144</v>
@@ -2243,7 +2560,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>1.2</v>
@@ -2268,7 +2585,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>8</v>
@@ -2289,6 +2606,70 @@
       <c r="G75" s="0" t="n">
         <f aca="false">ROUND(C75/E75*1000,2)</f>
         <v>197.71</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="0" t="n">
+        <v>0.144</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>0.673</v>
+      </c>
+      <c r="D79" s="1" t="n">
+        <v>5.6374</v>
+      </c>
+      <c r="E79" s="1" t="n">
+        <v>5.4213</v>
+      </c>
+      <c r="F79" s="0" t="n">
+        <f aca="false">ROUND(C79/D79*1000,2)</f>
+        <v>197.94</v>
+      </c>
+      <c r="G79" s="0" t="n">
+        <f aca="false">ROUND(C79/E79*1000,2)</f>
+        <v>143.8</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="D80" s="1" t="n">
+        <v>57.0173</v>
+      </c>
+      <c r="E80" s="1" t="n">
+        <v>50.1426</v>
+      </c>
+      <c r="F80" s="0" t="n">
+        <f aca="false">ROUND(C80/D80*1000,2)</f>
+        <v>98.22</v>
+      </c>
+      <c r="G80" s="0" t="n">
+        <f aca="false">ROUND(C80/E80*1000,2)</f>
+        <v>111.68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upgdated excel file in LibreOffice
</commit_message>
<xml_diff>
--- a/paper/images/results/TimesXMemory1_2BAM.xlsx
+++ b/paper/images/results/TimesXMemory1_2BAM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
   <si>
     <t xml:space="preserve">Algo</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Times x Memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBh</t>
   </si>
   <si>
     <t xml:space="preserve">Original</t>
@@ -110,14 +113,15 @@
       <color rgb="FFA9B7C6"/>
       <name val="DejaVu Sans Mono"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -178,18 +182,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -198,7 +202,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFFF38"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF7E0021"/>
@@ -219,7 +223,7 @@
       <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF38"/>
+      <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -235,14 +239,14 @@
       <rgbColor rgb="FFFFD7D7"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF83CAFF"/>
-      <rgbColor rgb="FF81D41A"/>
+      <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FFBF819E"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF579D1C"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -254,7 +258,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -318,12 +322,24 @@
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -376,11 +392,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="39982156"/>
-        <c:axId val="62623546"/>
+        <c:axId val="54763537"/>
+        <c:axId val="37094056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39982156"/>
+        <c:axId val="54763537"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -436,14 +452,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62623546"/>
+        <c:crossAx val="37094056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62623546"/>
+        <c:axId val="37094056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -480,7 +496,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39982156"/>
+        <c:crossAx val="54763537"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -520,14 +536,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -547,7 +563,7 @@
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Times x Memory (1.2 GB BAM File)</a:t>
+              <a:t>Times x Memory GBh (1.2 GB BAM File)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -607,39 +623,42 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$3</c:f>
+              <c:f>Sheet1!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Times x Memory</c:v>
+                  <c:v>MBh</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill>
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:srgbClr val="ffff00"/>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:srgbClr val="81d41a"/>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="3600000"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -667,24 +686,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$8</c:f>
+              <c:f>Sheet1!$E$4:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3968.22</c:v>
+                  <c:v>1.1023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2405.08</c:v>
+                  <c:v>0.6681</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2033.14</c:v>
+                  <c:v>0.5648</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>159.43</c:v>
+                  <c:v>0.0443</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>125.2</c:v>
+                  <c:v>0.0348</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -692,12 +711,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="34199797"/>
-        <c:axId val="77589560"/>
+        <c:axId val="76913927"/>
+        <c:axId val="86171590"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="34199797"/>
+        <c:axId val="76913927"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -753,14 +772,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77589560"/>
+        <c:crossAx val="86171590"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77589560"/>
+        <c:axId val="86171590"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -797,7 +816,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34199797"/>
+        <c:crossAx val="76913927"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -808,14 +827,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -915,11 +934,23 @@
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -972,12 +1003,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="52000376"/>
-        <c:axId val="51539058"/>
+        <c:axId val="11055459"/>
+        <c:axId val="85001440"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="52000376"/>
+        <c:axId val="11055459"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1033,14 +1064,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51539058"/>
+        <c:crossAx val="85001440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51539058"/>
+        <c:axId val="85001440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1105,7 +1136,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52000376"/>
+        <c:crossAx val="11055459"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1116,14 +1147,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1223,11 +1254,23 @@
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -1274,12 +1317,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="55761015"/>
-        <c:axId val="85189144"/>
+        <c:axId val="78194077"/>
+        <c:axId val="34140419"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="55761015"/>
+        <c:axId val="78194077"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1307,14 +1350,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85189144"/>
+        <c:crossAx val="34140419"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85189144"/>
+        <c:axId val="34140419"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1351,7 +1394,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55761015"/>
+        <c:crossAx val="78194077"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1383,14 +1426,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1410,7 +1453,7 @@
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>MB / second</a:t>
+              <a:t>MB / second (12core)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1498,11 +1541,23 @@
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -1566,11 +1621,23 @@
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -1611,12 +1678,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="57060530"/>
-        <c:axId val="91804926"/>
+        <c:axId val="53317959"/>
+        <c:axId val="83363313"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="57060530"/>
+        <c:axId val="53317959"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1644,14 +1711,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91804926"/>
+        <c:crossAx val="83363313"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91804926"/>
+        <c:axId val="83363313"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1688,7 +1755,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57060530"/>
+        <c:crossAx val="53317959"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1720,14 +1787,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1826,13 +1893,39 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$79:$A$80</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>BAM_144MB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BAM_1_2GB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$F$79:$F$80</c:f>
@@ -1840,7 +1933,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>197.94</c:v>
+                  <c:v>119.38</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>98.22</c:v>
@@ -1865,41 +1958,47 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="ff420e"/>
+              <a:srgbClr val="83caff"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:invertIfNegative val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$79:$A$80</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>BAM_144MB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BAM_1_2GB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$G$79:$G$80</c:f>
@@ -1907,7 +2006,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>143.8</c:v>
+                  <c:v>124.14</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>111.68</c:v>
@@ -1918,12 +2017,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="53961887"/>
-        <c:axId val="63720312"/>
+        <c:axId val="35867550"/>
+        <c:axId val="91834460"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="53961887"/>
+        <c:axId val="35867550"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1951,14 +2050,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63720312"/>
+        <c:crossAx val="91834460"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63720312"/>
+        <c:axId val="91834460"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1973,7 +2072,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1995,7 +2094,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53961887"/>
+        <c:crossAx val="35867550"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -2027,7 +2126,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -2045,9 +2144,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>690840</xdr:colOff>
+      <xdr:colOff>690480</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2056,7 +2155,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="386280" y="1816920"/>
-        <a:ext cx="5765400" cy="3241080"/>
+        <a:ext cx="5765040" cy="3240720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2075,9 +2174,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>507960</xdr:colOff>
+      <xdr:colOff>507600</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>76320</xdr:rowOff>
+      <xdr:rowOff>75960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2086,7 +2185,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="9151560" y="736560"/>
-        <a:ext cx="5771880" cy="3241080"/>
+        <a:ext cx="5771520" cy="3240720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2098,16 +2197,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>621720</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>86040</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>130680</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>694800</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>76320</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>203400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>104400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2115,8 +2214,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6082560" y="4475160"/>
-        <a:ext cx="5771520" cy="3241440"/>
+        <a:off x="15360480" y="601920"/>
+        <a:ext cx="5771160" cy="3241080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2128,16 +2227,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>656280</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>73800</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>156600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>64440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>726120</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>61920</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>226080</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2145,8 +2244,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6931080" y="7714080"/>
-        <a:ext cx="5768280" cy="3239280"/>
+        <a:off x="8873640" y="4128120"/>
+        <a:ext cx="5767920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2158,16 +2257,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>376920</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>28440</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>33120</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>438840</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>94320</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>114120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2175,8 +2274,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11536200" y="10269720"/>
-        <a:ext cx="5760360" cy="3241440"/>
+        <a:off x="9564120" y="8739720"/>
+        <a:ext cx="5760000" cy="3241080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2188,16 +2287,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>601920</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>74520</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>612360</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>36720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>663120</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>63000</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>673200</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2205,8 +2304,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5248800" y="13892040"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="9329400" y="12553560"/>
+        <a:ext cx="5759280" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2226,16 +2325,14 @@
   </sheetPr>
   <dimension ref="A3:G80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N49" activeCellId="0" sqref="N49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2251,10 +2348,13 @@
       <c r="D3" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E3" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>123.91</v>
@@ -2266,10 +2366,14 @@
         <f aca="false">ROUND(B4*C4, 2)</f>
         <v>3968.22</v>
       </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">ROUND(D4/3600*1, 4)</f>
+        <v>1.1023</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>75.1</v>
@@ -2281,10 +2385,14 @@
         <f aca="false">ROUND(B5*C5, 2)</f>
         <v>2405.08</v>
       </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">ROUND(D5/3600*1, 4)</f>
+        <v>0.6681</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>64.62</v>
@@ -2296,10 +2404,14 @@
         <f aca="false">ROUND(B6*C6, 2)</f>
         <v>2033.14</v>
       </c>
+      <c r="E6" s="0" t="n">
+        <f aca="false">ROUND(D6/3600*1, 4)</f>
+        <v>0.5648</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>34</v>
@@ -2311,10 +2423,14 @@
         <f aca="false">ROUND(B7*C7, 2)</f>
         <v>159.43</v>
       </c>
+      <c r="E7" s="0" t="n">
+        <f aca="false">ROUND(D7/3600*1, 4)</f>
+        <v>0.0443</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>26.7</v>
@@ -2325,6 +2441,10 @@
       <c r="D8" s="0" t="n">
         <f aca="false">ROUND(B8*C8, 2)</f>
         <v>125.2</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <f aca="false">ROUND(D8/3600*1, 4)</f>
+        <v>0.0348</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2343,7 +2463,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>3.938</v>
@@ -2358,7 +2478,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>4.19</v>
@@ -2373,7 +2493,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>3.43</v>
@@ -2388,7 +2508,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>3.4</v>
@@ -2403,7 +2523,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>4.68</v>
@@ -2418,7 +2538,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2437,7 +2557,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>9.128</v>
@@ -2452,7 +2572,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>8.98</v>
@@ -2467,7 +2587,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>8.8</v>
@@ -2482,7 +2602,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B52" s="1" t="n">
         <v>5.6374</v>
@@ -2497,7 +2617,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B53" s="1" t="n">
         <v>5.4213</v>
@@ -2512,30 +2632,30 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>0.144</v>
@@ -2560,7 +2680,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>1.2</v>
@@ -2585,7 +2705,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>8</v>
@@ -2609,26 +2729,32 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="B78" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>16</v>
+      </c>
       <c r="B79" s="0" t="n">
         <v>0.144</v>
       </c>
@@ -2642,15 +2768,18 @@
         <v>5.4213</v>
       </c>
       <c r="F79" s="0" t="n">
-        <f aca="false">ROUND(C79/D79*1000,2)</f>
-        <v>197.94</v>
+        <f aca="false">ROUND(C79/D79*1000, 2)</f>
+        <v>119.38</v>
       </c>
       <c r="G79" s="0" t="n">
         <f aca="false">ROUND(C79/E79*1000,2)</f>
-        <v>143.8</v>
+        <v>124.14</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>17</v>
+      </c>
       <c r="B80" s="0" t="n">
         <v>1.2</v>
       </c>
@@ -2664,7 +2793,7 @@
         <v>50.1426</v>
       </c>
       <c r="F80" s="0" t="n">
-        <f aca="false">ROUND(C80/D80*1000,2)</f>
+        <f aca="false">ROUND(C80/D80*1000, 2)</f>
         <v>98.22</v>
       </c>
       <c r="G80" s="0" t="n">

</xml_diff>

<commit_message>
Graphs and value updates
</commit_message>
<xml_diff>
--- a/paper/images/results/TimesXMemory1_2BAM.xlsx
+++ b/paper/images/results/TimesXMemory1_2BAM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
   <si>
     <t xml:space="preserve">Algo</t>
   </si>
@@ -70,6 +70,12 @@
     <t xml:space="preserve">Time Par</t>
   </si>
   <si>
+    <t xml:space="preserve">Time Orig(Opt)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElPrep SBA</t>
+  </si>
+  <si>
     <t xml:space="preserve">BAM_144MB</t>
   </si>
   <si>
@@ -77,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">BAM_8GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?</t>
   </si>
 </sst>
 </file>
@@ -116,12 +125,12 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -173,7 +182,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -183,6 +192,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -202,7 +215,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF38"/>
+      <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF7E0021"/>
@@ -223,7 +236,7 @@
       <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFFF38"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -243,7 +256,7 @@
       <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF3465A4"/>
       <rgbColor rgb="FFBF819E"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF579D1C"/>
@@ -392,11 +405,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="54763537"/>
-        <c:axId val="37094056"/>
+        <c:axId val="2506823"/>
+        <c:axId val="47628419"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="54763537"/>
+        <c:axId val="2506823"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,14 +465,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37094056"/>
+        <c:crossAx val="47628419"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37094056"/>
+        <c:axId val="47628419"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,7 +509,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54763537"/>
+        <c:crossAx val="2506823"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -642,6 +655,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -711,12 +725,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="76913927"/>
-        <c:axId val="86171590"/>
+        <c:axId val="82913342"/>
+        <c:axId val="91868285"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="76913927"/>
+        <c:axId val="82913342"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -772,14 +786,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86171590"/>
+        <c:crossAx val="91868285"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86171590"/>
+        <c:axId val="91868285"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -816,7 +830,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76913927"/>
+        <c:crossAx val="82913342"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1003,12 +1017,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="11055459"/>
-        <c:axId val="85001440"/>
+        <c:axId val="65182678"/>
+        <c:axId val="97289176"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="11055459"/>
+        <c:axId val="65182678"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1064,14 +1078,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85001440"/>
+        <c:crossAx val="97289176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85001440"/>
+        <c:axId val="97289176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1136,7 +1150,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11055459"/>
+        <c:crossAx val="65182678"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1317,12 +1331,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="78194077"/>
-        <c:axId val="34140419"/>
+        <c:axId val="1171714"/>
+        <c:axId val="24755662"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="78194077"/>
+        <c:axId val="1171714"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1350,14 +1364,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34140419"/>
+        <c:crossAx val="24755662"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34140419"/>
+        <c:axId val="24755662"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1394,7 +1408,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78194077"/>
+        <c:crossAx val="1171714"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1453,7 +1467,7 @@
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>MB / second (12core)</a:t>
+              <a:t>Second/GB(12core)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1513,7 +1527,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$72</c:f>
+              <c:f>Sheet1!$G$72:$G$72</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1579,18 +1593,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$73:$F$75</c:f>
+              <c:f>Sheet1!$G$73:$G$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>197.94</c:v>
+                  <c:v>5.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>164.71</c:v>
+                  <c:v>6.07</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>185</c:v>
+                  <c:v>5.41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1601,7 +1615,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$72</c:f>
+              <c:f>Sheet1!$H$72:$H$72</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1659,18 +1673,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$73:$G$75</c:f>
+              <c:f>Sheet1!$H$73:$H$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>143.8</c:v>
+                  <c:v>6.95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>209.74</c:v>
+                  <c:v>4.77</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>197.71</c:v>
+                  <c:v>5.06</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1678,12 +1692,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="53317959"/>
-        <c:axId val="83363313"/>
+        <c:axId val="27575680"/>
+        <c:axId val="78450618"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="53317959"/>
+        <c:axId val="27575680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1711,14 +1725,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83363313"/>
+        <c:crossAx val="78450618"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83363313"/>
+        <c:axId val="78450618"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1755,7 +1769,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53317959"/>
+        <c:crossAx val="27575680"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1893,6 +1907,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1966,6 +1981,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -2017,12 +2033,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="35867550"/>
-        <c:axId val="91834460"/>
+        <c:axId val="48136201"/>
+        <c:axId val="54204089"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="35867550"/>
+        <c:axId val="48136201"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2050,14 +2066,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91834460"/>
+        <c:crossAx val="54204089"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91834460"/>
+        <c:axId val="54204089"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2094,7 +2110,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35867550"/>
+        <c:crossAx val="48136201"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -2133,6 +2149,723 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sec / GB</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="11"/>
+      <c:rotY val="25"/>
+      <c:rAngAx val="1"/>
+      <c:perspective val="40"/>
+    </c:view3D>
+    <c:floor>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="cccccc"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$72</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Compact</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$73:$B$75</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$73:$G$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.07</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$72</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Compact Par</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffff00"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$73:$B$75</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$73:$H$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.06</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$72</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ElPrep SBA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3465a4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$73:$B$75</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$73:$I$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.54</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:shape val="box"/>
+        <c:axId val="59578540"/>
+        <c:axId val="57767645"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="59578540"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="57767645"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="57767645"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="59578540"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Times x Memory 4 core (0.144 GB BAM)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="11"/>
+      <c:rotY val="25"/>
+      <c:rAngAx val="1"/>
+      <c:perspective val="40"/>
+    </c:view3D>
+    <c:floor>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="cccccc"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Times x Memory</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$49:$A$53</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Buffered</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>StreamByteArray</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Compact</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Compact Par</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$49:$D$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>21.23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:shape val="box"/>
+        <c:axId val="6588691"/>
+        <c:axId val="39301319"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="6588691"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="39301319"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="39301319"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="6588691"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -2144,9 +2877,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>690480</xdr:colOff>
+      <xdr:colOff>690120</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>18360</xdr:rowOff>
+      <xdr:rowOff>18000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2155,7 +2888,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="386280" y="1816920"/>
-        <a:ext cx="5765040" cy="3240720"/>
+        <a:ext cx="5767200" cy="3240360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2174,9 +2907,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>507600</xdr:colOff>
+      <xdr:colOff>507240</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>75960</xdr:rowOff>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2184,8 +2917,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9151560" y="736560"/>
-        <a:ext cx="5771520" cy="3240720"/>
+        <a:off x="9159120" y="736560"/>
+        <a:ext cx="5780160" cy="3240360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2204,9 +2937,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>203400</xdr:colOff>
+      <xdr:colOff>203040</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>104400</xdr:rowOff>
+      <xdr:rowOff>104040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2214,8 +2947,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15360480" y="601920"/>
-        <a:ext cx="5771160" cy="3241080"/>
+        <a:off x="15378120" y="601920"/>
+        <a:ext cx="5779800" cy="3240720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2234,9 +2967,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>226080</xdr:colOff>
+      <xdr:colOff>225720</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>51840</xdr:rowOff>
+      <xdr:rowOff>51480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2244,8 +2977,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8873640" y="4128120"/>
-        <a:ext cx="5767920" cy="3238920"/>
+        <a:off x="8881200" y="4128120"/>
+        <a:ext cx="5776560" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2258,15 +2991,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>33120</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>124200</xdr:rowOff>
+      <xdr:colOff>337320</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>28440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>94320</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:colOff>398160</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>18000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2274,8 +3007,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9564120" y="8739720"/>
-        <a:ext cx="5760000" cy="3241080"/>
+        <a:off x="9877320" y="7668720"/>
+        <a:ext cx="5768280" cy="3240720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2294,9 +3027,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>673200</xdr:colOff>
+      <xdr:colOff>672840</xdr:colOff>
       <xdr:row>97</xdr:row>
-      <xdr:rowOff>24840</xdr:rowOff>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2304,12 +3037,72 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9329400" y="12553560"/>
-        <a:ext cx="5759280" cy="3239280"/>
+        <a:off x="9336960" y="12553560"/>
+        <a:ext cx="5767920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>547920</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>105120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>63720</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>95760</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="3843360" y="13922640"/>
+        <a:ext cx="5760360" cy="3241800"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>36360</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>36000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>88560</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>24480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="5499720" y="7676280"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2323,13 +3116,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:G80"/>
+  <dimension ref="A3:I80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.17"/>
@@ -2647,15 +3440,21 @@
         <v>15</v>
       </c>
       <c r="F72" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G72" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G72" s="0" t="s">
+      <c r="H72" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="I72" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>0.144</v>
@@ -2669,18 +3468,25 @@
       <c r="E73" s="0" t="n">
         <v>4.68</v>
       </c>
-      <c r="F73" s="0" t="n">
-        <f aca="false">ROUND(C73/D73*1000,2)</f>
-        <v>197.94</v>
+      <c r="F73" s="3" t="n">
+        <v>3.43</v>
       </c>
       <c r="G73" s="0" t="n">
-        <f aca="false">ROUND(C73/E73*1000,2)</f>
-        <v>143.8</v>
+        <f aca="false">ROUND(D73/C73,2)</f>
+        <v>5.05</v>
+      </c>
+      <c r="H73" s="0" t="n">
+        <f aca="false">ROUND(E73/C73,2)</f>
+        <v>6.95</v>
+      </c>
+      <c r="I73" s="0" t="n">
+        <f aca="false">ROUND(F73/C73,2)</f>
+        <v>5.1</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>1.2</v>
@@ -2694,18 +3500,25 @@
       <c r="E74" s="0" t="n">
         <v>26.7</v>
       </c>
-      <c r="F74" s="0" t="n">
-        <f aca="false">ROUND(C74/D74*1000,2)</f>
-        <v>164.71</v>
+      <c r="F74" s="3" t="n">
+        <v>64.62</v>
       </c>
       <c r="G74" s="0" t="n">
-        <f aca="false">ROUND(C74/E74*1000,2)</f>
-        <v>209.74</v>
+        <f aca="false">ROUND(D74/C74,2)</f>
+        <v>6.07</v>
+      </c>
+      <c r="H74" s="0" t="n">
+        <f aca="false">ROUND(E74/C74,2)</f>
+        <v>4.77</v>
+      </c>
+      <c r="I74" s="0" t="n">
+        <f aca="false">ROUND(F74/C74,2)</f>
+        <v>11.54</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>8</v>
@@ -2719,13 +3532,20 @@
       <c r="E75" s="0" t="n">
         <v>131</v>
       </c>
-      <c r="F75" s="0" t="n">
-        <f aca="false">ROUND(C75/D75*1000,2)</f>
-        <v>185</v>
+      <c r="F75" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="G75" s="0" t="n">
-        <f aca="false">ROUND(C75/E75*1000,2)</f>
-        <v>197.71</v>
+        <f aca="false">ROUND(D75/C75,2)</f>
+        <v>5.41</v>
+      </c>
+      <c r="H75" s="0" t="n">
+        <f aca="false">ROUND(E75/C75,2)</f>
+        <v>5.06</v>
+      </c>
+      <c r="I75" s="0" t="e">
+        <f aca="false">ROUND(F75/C75,2)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2753,7 +3573,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>0.144</v>
@@ -2778,7 +3598,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>1.2</v>

</xml_diff>

<commit_message>
Adds clarifications around per row instance cost.
</commit_message>
<xml_diff>
--- a/paper/images/results/TimesXMemory1_2BAM.xlsx
+++ b/paper/images/results/TimesXMemory1_2BAM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
     <t xml:space="preserve">Algo</t>
   </si>
@@ -87,6 +87,54 @@
   <si>
     <t xml:space="preserve">?</t>
   </si>
+  <si>
+    <t xml:space="preserve">Instance size Estimations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instance Type name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamAlignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MapQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cigar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rnext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pnext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Underlying String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
 </sst>
 </file>
 
@@ -125,12 +173,12 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -182,7 +230,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -192,10 +240,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -232,14 +276,14 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF0084D1"/>
       <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF38"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FFC5000B"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
@@ -252,19 +296,19 @@
       <rgbColor rgb="FFFFD7D7"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF83CAFF"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFAECF00"/>
       <rgbColor rgb="FFFFD320"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF950E"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF3465A4"/>
       <rgbColor rgb="FFBF819E"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF579D1C"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF314004"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF4B1F6F"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
@@ -405,11 +449,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="2506823"/>
-        <c:axId val="47628419"/>
+        <c:axId val="94755717"/>
+        <c:axId val="96242640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2506823"/>
+        <c:axId val="94755717"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -465,14 +509,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47628419"/>
+        <c:crossAx val="96242640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47628419"/>
+        <c:axId val="96242640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -509,7 +553,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2506823"/>
+        <c:crossAx val="94755717"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -725,12 +769,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="82913342"/>
-        <c:axId val="91868285"/>
+        <c:axId val="36897946"/>
+        <c:axId val="28696400"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="82913342"/>
+        <c:axId val="36897946"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -786,14 +830,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91868285"/>
+        <c:crossAx val="28696400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91868285"/>
+        <c:axId val="28696400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,7 +874,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82913342"/>
+        <c:crossAx val="36897946"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1017,12 +1061,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="65182678"/>
-        <c:axId val="97289176"/>
+        <c:axId val="27402487"/>
+        <c:axId val="70583766"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="65182678"/>
+        <c:axId val="27402487"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1078,14 +1122,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97289176"/>
+        <c:crossAx val="70583766"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97289176"/>
+        <c:axId val="70583766"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1150,7 +1194,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65182678"/>
+        <c:crossAx val="27402487"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1331,12 +1375,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="1171714"/>
-        <c:axId val="24755662"/>
+        <c:axId val="46092887"/>
+        <c:axId val="24018853"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1171714"/>
+        <c:axId val="46092887"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1364,14 +1408,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24755662"/>
+        <c:crossAx val="24018853"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="24755662"/>
+        <c:axId val="24018853"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1408,7 +1452,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1171714"/>
+        <c:crossAx val="46092887"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1692,12 +1736,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="27575680"/>
-        <c:axId val="78450618"/>
+        <c:axId val="34694733"/>
+        <c:axId val="1129724"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="27575680"/>
+        <c:axId val="34694733"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1725,14 +1769,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78450618"/>
+        <c:crossAx val="1129724"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78450618"/>
+        <c:axId val="1129724"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1769,7 +1813,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27575680"/>
+        <c:crossAx val="34694733"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -2033,12 +2077,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="48136201"/>
-        <c:axId val="54204089"/>
+        <c:axId val="93515432"/>
+        <c:axId val="9177617"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="48136201"/>
+        <c:axId val="93515432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2066,14 +2110,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54204089"/>
+        <c:crossAx val="9177617"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54204089"/>
+        <c:axId val="9177617"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2110,7 +2154,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48136201"/>
+        <c:crossAx val="93515432"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -2250,6 +2294,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -2331,6 +2376,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -2412,6 +2458,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -2466,12 +2513,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="59578540"/>
-        <c:axId val="57767645"/>
+        <c:axId val="10800039"/>
+        <c:axId val="66527253"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="59578540"/>
+        <c:axId val="10800039"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2499,14 +2546,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57767645"/>
+        <c:crossAx val="66527253"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57767645"/>
+        <c:axId val="66527253"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2521,7 +2568,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2543,7 +2590,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59578540"/>
+        <c:crossAx val="10800039"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -2575,7 +2622,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -2681,6 +2728,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -2750,12 +2798,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="6588691"/>
-        <c:axId val="39301319"/>
+        <c:axId val="1671765"/>
+        <c:axId val="67325528"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="6588691"/>
+        <c:axId val="1671765"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2783,14 +2831,1272 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39301319"/>
+        <c:crossAx val="67325528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39301319"/>
+        <c:axId val="67325528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1671765"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Memory Bookeeping</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="11"/>
+      <c:rotY val="25"/>
+      <c:rAngAx val="1"/>
+      <c:perspective val="40"/>
+    </c:view3D>
+    <c:floor>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="cccccc"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:bar3DChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$113</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SamAlignment</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$112:$D$112</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ElPrep (189 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Compact (39 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chunked Comp (33 bytes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$113:$D$113</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$114</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>QName</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$112:$D$112</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ElPrep (189 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Compact (39 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chunked Comp (33 bytes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$114:$D$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$115</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Flag</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$112:$D$112</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ElPrep (189 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Compact (39 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chunked Comp (33 bytes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$115:$D$115</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$116</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rname</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$112:$D$112</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ElPrep (189 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Compact (39 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chunked Comp (33 bytes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$116:$D$116</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$117</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7e0021"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$112:$D$112</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ElPrep (189 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Compact (39 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chunked Comp (33 bytes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$117:$D$117</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$118</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MapQ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="83caff"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$112:$D$112</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ElPrep (189 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Compact (39 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chunked Comp (33 bytes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$118:$D$118</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$119</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cigar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="314004"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$112:$D$112</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ElPrep (189 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Compact (39 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chunked Comp (33 bytes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$119:$D$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$120</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rnext</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="aecf00"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$112:$D$112</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ElPrep (189 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Compact (39 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chunked Comp (33 bytes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$120:$D$120</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$121</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pnext</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4b1f6f"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$112:$D$112</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ElPrep (189 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Compact (39 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chunked Comp (33 bytes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$121:$D$121</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$122</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TLen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff950e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$112:$D$112</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ElPrep (189 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Compact (39 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chunked Comp (33 bytes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$122:$D$122</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$123</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Seq</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="c5000b"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$112:$D$112</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ElPrep (189 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Compact (39 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chunked Comp (33 bytes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$123:$D$123</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$124</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Qual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0084d1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="3465a4"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="3465a4"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$112:$D$112</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ElPrep (189 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Compact (39 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chunked Comp (33 bytes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$124:$D$124</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$125</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Underlying String</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$112:$D$112</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ElPrep (189 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Compact (39 bytes)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chunked Comp (33 bytes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$125:$D$125</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:shape val="box"/>
+        <c:axId val="22880914"/>
+        <c:axId val="18215756"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="22880914"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="18215756"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="18215756"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2827,7 +4133,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6588691"/>
+        <c:crossAx val="22880914"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -2877,9 +4183,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>690120</xdr:colOff>
+      <xdr:colOff>261720</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2888,7 +4194,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="386280" y="1816920"/>
-        <a:ext cx="5767200" cy="3240360"/>
+        <a:ext cx="5769360" cy="3240000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2901,15 +4207,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>434520</xdr:colOff>
+      <xdr:colOff>434880</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>86400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>507240</xdr:colOff>
+      <xdr:colOff>506880</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:rowOff>75240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2917,8 +4223,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9159120" y="736560"/>
-        <a:ext cx="5780160" cy="3240360"/>
+        <a:off x="9595080" y="736560"/>
+        <a:ext cx="5788440" cy="3240000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2931,9 +4237,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>130680</xdr:colOff>
+      <xdr:colOff>131040</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:rowOff>114840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
@@ -2947,8 +4253,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15378120" y="601920"/>
-        <a:ext cx="5779800" cy="3240720"/>
+        <a:off x="15824160" y="602280"/>
+        <a:ext cx="5788440" cy="3240360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2961,13 +4267,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>156600</xdr:colOff>
+      <xdr:colOff>156960</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>64440</xdr:rowOff>
+      <xdr:rowOff>64800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>225720</xdr:colOff>
+      <xdr:colOff>225360</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>51480</xdr:rowOff>
     </xdr:to>
@@ -2977,8 +4283,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8881200" y="4128120"/>
-        <a:ext cx="5776560" cy="3238560"/>
+        <a:off x="9317160" y="4128480"/>
+        <a:ext cx="5784840" cy="3238200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2997,9 +4303,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>398160</xdr:colOff>
+      <xdr:colOff>397800</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3007,8 +4313,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9877320" y="7668720"/>
-        <a:ext cx="5768280" cy="3240720"/>
+        <a:off x="10314360" y="7668720"/>
+        <a:ext cx="5776560" cy="3240360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3021,13 +4327,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>612360</xdr:colOff>
+      <xdr:colOff>612720</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>672840</xdr:colOff>
+      <xdr:colOff>672480</xdr:colOff>
       <xdr:row>97</xdr:row>
       <xdr:rowOff>24480</xdr:rowOff>
     </xdr:to>
@@ -3037,8 +4343,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9336960" y="12553560"/>
-        <a:ext cx="5767920" cy="3238920"/>
+        <a:off x="9772920" y="12553920"/>
+        <a:ext cx="5776200" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3056,10 +4362,10 @@
       <xdr:rowOff>105120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>63720</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>452160</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:rowOff>95400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3067,8 +4373,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3843360" y="13922640"/>
-        <a:ext cx="5760360" cy="3241800"/>
+        <a:off x="3844800" y="13922640"/>
+        <a:ext cx="5767560" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3089,7 +4395,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>88560</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:rowOff>24120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3097,12 +4403,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5499720" y="7676280"/>
+        <a:off x="5930280" y="7676280"/>
+        <a:ext cx="5768280" cy="3239280"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>203400</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>102960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>246960</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="7730640" y="17821800"/>
         <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3116,16 +4452,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:I80"/>
+  <dimension ref="A3:I126"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D112" activeCellId="0" sqref="D112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.64"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3468,7 +4805,7 @@
       <c r="E73" s="0" t="n">
         <v>4.68</v>
       </c>
-      <c r="F73" s="3" t="n">
+      <c r="F73" s="2" t="n">
         <v>3.43</v>
       </c>
       <c r="G73" s="0" t="n">
@@ -3500,7 +4837,7 @@
       <c r="E74" s="0" t="n">
         <v>26.7</v>
       </c>
-      <c r="F74" s="3" t="n">
+      <c r="F74" s="2" t="n">
         <v>64.62</v>
       </c>
       <c r="G74" s="0" t="n">
@@ -3619,6 +4956,227 @@
       <c r="G80" s="0" t="n">
         <f aca="false">ROUND(C80/E80*1000,2)</f>
         <v>111.68</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B112" s="0" t="str">
+        <f aca="false"> "ElPrep (" &amp; $B126 &amp; " bytes)"</f>
+        <v>ElPrep (189 bytes)</v>
+      </c>
+      <c r="C112" s="0" t="str">
+        <f aca="false"> "Compact (" &amp; $C126 &amp; " bytes)"</f>
+        <v>Compact (39 bytes)</v>
+      </c>
+      <c r="D112" s="0" t="str">
+        <f aca="false"> "Chunked Comp (" &amp; $D126 &amp; " bytes)"</f>
+        <v>Chunked Comp (33 bytes)</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B113" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C113" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D113" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B114" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C114" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D114" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B115" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D115" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B116" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C116" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D116" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B117" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D117" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B118" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D118" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B119" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C119" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D119" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B120" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C120" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D120" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B121" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C121" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D121" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B122" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C122" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D122" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B123" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C123" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D123" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B124" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C124" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D124" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B125" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C125" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D125" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B126" s="0" t="n">
+        <f aca="false">SUM(B113:B125)</f>
+        <v>189</v>
+      </c>
+      <c r="C126" s="0" t="n">
+        <f aca="false">SUM(C113:C125)</f>
+        <v>39</v>
+      </c>
+      <c r="D126" s="0" t="n">
+        <f aca="false">SUM(D113:D125)</f>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated graphs / remove legends / change "times" -> "time"
</commit_message>
<xml_diff>
--- a/paper/images/results/TimesXMemory1_2BAM.xlsx
+++ b/paper/images/results/TimesXMemory1_2BAM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
   <si>
     <t xml:space="preserve">Algo</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Memory</t>
   </si>
   <si>
-    <t xml:space="preserve">Times x Memory</t>
+    <t xml:space="preserve">Time x Memory</t>
   </si>
   <si>
     <t xml:space="preserve">MBh</t>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Compact Par</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Times x Memory</t>
   </si>
   <si>
     <t xml:space="preserve">4c</t>
@@ -265,7 +268,7 @@
       <rgbColor rgb="FF7E0021"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFCCCCCC"/>
@@ -277,7 +280,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0084D1"/>
-      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF83CAFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF38"/>
@@ -295,13 +298,13 @@
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFD7D7"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF83CAFF"/>
+      <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FFAECF00"/>
       <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF950E"/>
       <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF3465A4"/>
-      <rgbColor rgb="FFBF819E"/>
+      <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF579D1C"/>
       <rgbColor rgb="FF003300"/>
@@ -315,7 +318,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -335,7 +338,7 @@
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Times x Memory (1.2 GB BAM File)</a:t>
+              <a:t>Time x Memory (1.2 GB BAM File)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -363,7 +366,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Times x Memory</c:v>
+                  <c:v>Time x Memory</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -449,11 +452,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="26654033"/>
-        <c:axId val="25011286"/>
+        <c:axId val="34763032"/>
+        <c:axId val="10359596"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="26654033"/>
+        <c:axId val="34763032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -509,14 +512,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25011286"/>
+        <c:crossAx val="10359596"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="25011286"/>
+        <c:axId val="10359596"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,7 +556,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26654033"/>
+        <c:crossAx val="34763032"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -565,27 +568,6 @@
         </a:ln>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
@@ -600,7 +582,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -769,12 +751,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="31437059"/>
-        <c:axId val="34146932"/>
+        <c:axId val="13064110"/>
+        <c:axId val="4128239"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="31437059"/>
+        <c:axId val="13064110"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,14 +812,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34146932"/>
+        <c:crossAx val="4128239"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34146932"/>
+        <c:axId val="4128239"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,7 +856,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31437059"/>
+        <c:crossAx val="13064110"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -892,7 +874,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1061,12 +1043,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="70735891"/>
-        <c:axId val="23718032"/>
+        <c:axId val="39798048"/>
+        <c:axId val="83880732"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="70735891"/>
+        <c:axId val="39798048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1122,14 +1104,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23718032"/>
+        <c:crossAx val="83880732"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23718032"/>
+        <c:axId val="83880732"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1194,7 +1176,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70735891"/>
+        <c:crossAx val="39798048"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1212,286 +1194,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Times x Memory 4c (144 MB BAM File)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="11"/>
-      <c:rotY val="25"/>
-      <c:rAngAx val="1"/>
-      <c:perspective val="40"/>
-    </c:view3D>
-    <c:floor>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="cccccc"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:floor>
-    <c:sideWall>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:sideWall>
-    <c:backWall>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:backWall>
-    <c:plotArea>
-      <c:bar3DChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$48</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Times x Memory</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="bf819e"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$49:$A$52</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Original</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Buffered</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>StreamByteArray</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Compact</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$49:$D$52</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>21.23</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20.89</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20.02</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.42</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:gapWidth val="100"/>
-        <c:shape val="box"/>
-        <c:axId val="90504414"/>
-        <c:axId val="37780551"/>
-        <c:axId val="0"/>
-      </c:bar3DChart>
-      <c:catAx>
-        <c:axId val="90504414"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="37780551"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="37780551"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="90504414"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1736,12 +1439,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="53912878"/>
-        <c:axId val="58818851"/>
+        <c:axId val="24085062"/>
+        <c:axId val="27023087"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="53912878"/>
+        <c:axId val="24085062"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1769,14 +1472,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58818851"/>
+        <c:crossAx val="27023087"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58818851"/>
+        <c:axId val="27023087"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1813,7 +1516,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53912878"/>
+        <c:crossAx val="24085062"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -1852,7 +1555,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2077,12 +1780,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="87609476"/>
-        <c:axId val="56093910"/>
+        <c:axId val="78590946"/>
+        <c:axId val="82152473"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="87609476"/>
+        <c:axId val="78590946"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2110,14 +1813,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56093910"/>
+        <c:crossAx val="82152473"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56093910"/>
+        <c:axId val="82152473"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2154,7 +1857,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87609476"/>
+        <c:crossAx val="78590946"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -2193,7 +1896,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2513,12 +2216,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="18557661"/>
-        <c:axId val="97892576"/>
+        <c:axId val="79388036"/>
+        <c:axId val="68432600"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="18557661"/>
+        <c:axId val="79388036"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2546,14 +2249,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97892576"/>
+        <c:crossAx val="68432600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97892576"/>
+        <c:axId val="68432600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2590,7 +2293,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18557661"/>
+        <c:crossAx val="79388036"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
@@ -2629,7 +2332,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2649,7 +2352,7 @@
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Times x Memory 4 core (0.144 GB BAM)</a:t>
+              <a:t>Time x Memory 4 core (0.144 GB BAM)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2798,12 +2501,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="33733414"/>
-        <c:axId val="28562263"/>
+        <c:axId val="63214362"/>
+        <c:axId val="19315845"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="33733414"/>
+        <c:axId val="63214362"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2831,14 +2534,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28562263"/>
+        <c:crossAx val="19315845"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28562263"/>
+        <c:axId val="19315845"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2875,31 +2578,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33733414"/>
+        <c:crossAx val="63214362"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
@@ -2914,7 +2596,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3014,6 +2696,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -3093,6 +2776,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -3172,6 +2856,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -3251,6 +2936,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -3330,6 +3016,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -3409,6 +3096,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -3488,6 +3176,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -3567,6 +3256,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -3646,6 +3336,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -3725,6 +3416,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -3804,6 +3496,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -3895,8 +3588,10 @@
             </c:spPr>
           </c:dPt>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
               <c:txPr>
                 <a:bodyPr/>
                 <a:lstStyle/>
@@ -4000,6 +3695,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -4057,12 +3753,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="86538421"/>
-        <c:axId val="12105522"/>
+        <c:axId val="12392641"/>
+        <c:axId val="15718750"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="86538421"/>
+        <c:axId val="12392641"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4090,14 +3786,426 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12105522"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="15718750"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="12105522"/>
+        <c:axId val="15718750"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="12392641"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Time x Memory (1.2 GB BAM File)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="8"/>
+      <c:rotY val="25"/>
+      <c:rAngAx val="1"/>
+      <c:perspective val="40"/>
+    </c:view3D>
+    <c:floor>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="3465a4"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time x Memory</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:srgbClr val="ffff00"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:srgbClr val="81d41a"/>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="3600000"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:srgbClr val="ffff00"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:srgbClr val="81d41a"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="3600000"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:srgbClr val="ffff00"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:srgbClr val="81d41a"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="3600000"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:srgbClr val="ffff00"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:srgbClr val="81d41a"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="3600000"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$4:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Buffered</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>StreamByteArray</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Compact</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Compact Par</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3968.22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2405.08</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2033.14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>159.43</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:shape val="box"/>
+        <c:axId val="98517113"/>
+        <c:axId val="66376297"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="98517113"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="66376297"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="66376297"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4134,31 +4242,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86538421"/>
+        <c:crossAx val="98517113"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
@@ -4184,9 +4271,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>261720</xdr:colOff>
+      <xdr:colOff>261360</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
+      <xdr:rowOff>17280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4195,7 +4282,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="386280" y="1816920"/>
-        <a:ext cx="5769360" cy="3240000"/>
+        <a:ext cx="5770080" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4207,16 +4294,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>434880</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>267480</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>28800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>506880</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>75240</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>339120</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>17280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4224,8 +4311,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9595080" y="736560"/>
-        <a:ext cx="5788440" cy="3240000"/>
+        <a:off x="15977160" y="4417920"/>
+        <a:ext cx="5796720" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4244,9 +4331,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>203040</xdr:colOff>
+      <xdr:colOff>202680</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4254,42 +4341,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15824160" y="602280"/>
-        <a:ext cx="5788440" cy="3240360"/>
+        <a:off x="15840720" y="602280"/>
+        <a:ext cx="5796720" cy="3240000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>156960</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>64800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>225360</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>51480</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name=""/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="9317160" y="4128480"/>
-        <a:ext cx="5784840" cy="3238200"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4304,22 +4361,22 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>397800</xdr:colOff>
+      <xdr:colOff>397440</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
+      <xdr:rowOff>17280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name=""/>
+        <xdr:cNvPr id="3" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10314360" y="7668720"/>
-        <a:ext cx="5776560" cy="3240360"/>
+        <a:off x="10321920" y="7668720"/>
+        <a:ext cx="5785200" cy="3240000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4334,22 +4391,22 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>672480</xdr:colOff>
+      <xdr:colOff>672120</xdr:colOff>
       <xdr:row>97</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:rowOff>24120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvPr id="4" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9772920" y="12553920"/>
-        <a:ext cx="5776200" cy="3238560"/>
+        <a:off x="9779400" y="12553920"/>
+        <a:ext cx="5784480" cy="3238200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4364,9 +4421,39 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>452160</xdr:colOff>
+      <xdr:colOff>451800</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:rowOff>95040</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="3845880" y="13922640"/>
+        <a:ext cx="5772600" cy="3241080"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>442080</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>38520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>491760</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4374,42 +4461,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3844800" y="13922640"/>
-        <a:ext cx="5767560" cy="3241440"/>
+        <a:off x="7155000" y="4102200"/>
+        <a:ext cx="5775120" cy="3232080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>36360</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>88560</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>24120</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name=""/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="5930280" y="7676280"/>
-        <a:ext cx="5768280" cy="3239280"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4424,9 +4481,39 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>98640</xdr:colOff>
+      <xdr:colOff>98280</xdr:colOff>
       <xdr:row>137</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>84960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="7734240" y="17821800"/>
+        <a:ext cx="8073720" cy="4533840"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>243360</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>64800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>739080</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>53280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4434,8 +4521,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7730640" y="17821800"/>
-        <a:ext cx="8061120" cy="4534200"/>
+        <a:off x="6956280" y="389880"/>
+        <a:ext cx="5403240" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4455,11 +4542,11 @@
   </sheetPr>
   <dimension ref="A3:I126"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N105" activeCellId="0" sqref="N105"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P26" activeCellId="0" sqref="P26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.17"/>
@@ -4589,7 +4676,7 @@
         <v>2</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4669,7 +4756,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4683,7 +4770,7 @@
         <v>2</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4763,22 +4850,22 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G72" s="0" t="s">
         <v>8</v>
@@ -4787,12 +4874,12 @@
         <v>9</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>0.144</v>
@@ -4824,7 +4911,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>1.2</v>
@@ -4856,7 +4943,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>8</v>
@@ -4871,7 +4958,7 @@
         <v>131</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G75" s="0" t="n">
         <f aca="false">ROUND(D75/C75,2)</f>
@@ -4888,19 +4975,19 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F78" s="0" t="s">
         <v>8</v>
@@ -4911,7 +4998,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>0.144</v>
@@ -4936,7 +5023,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>1.2</v>
@@ -4961,29 +5048,29 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B112" s="0" t="str">
-        <f aca="false"> "ElPrep (" &amp; $B126 &amp; " bytes)"</f>
+        <f aca="false">"ElPrep (" &amp; $B126 &amp; " bytes)"</f>
         <v>ElPrep (189 bytes)</v>
       </c>
       <c r="C112" s="0" t="str">
-        <f aca="false"> "Compact (" &amp; $C126 &amp; " bytes)"</f>
+        <f aca="false">"Compact (" &amp; $C126 &amp; " bytes)"</f>
         <v>Compact (39 bytes)</v>
       </c>
       <c r="D112" s="0" t="str">
-        <f aca="false"> "Chunked Comp (" &amp; $D126 &amp; " bytes)"</f>
+        <f aca="false">"Chunked Comp (" &amp; $D126 &amp; " bytes)"</f>
         <v>Chunked Comp (33 bytes)</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B113" s="0" t="n">
         <v>6</v>
@@ -4997,7 +5084,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B114" s="0" t="n">
         <v>24</v>
@@ -5011,7 +5098,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B115" s="0" t="n">
         <v>2</v>
@@ -5025,7 +5112,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B116" s="0" t="n">
         <v>24</v>
@@ -5039,7 +5126,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B117" s="0" t="n">
         <v>4</v>
@@ -5053,7 +5140,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B118" s="0" t="n">
         <v>1</v>
@@ -5067,7 +5154,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B119" s="0" t="n">
         <v>24</v>
@@ -5081,7 +5168,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B120" s="0" t="n">
         <v>24</v>
@@ -5095,7 +5182,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B121" s="0" t="n">
         <v>4</v>
@@ -5109,7 +5196,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B122" s="0" t="n">
         <v>4</v>
@@ -5123,7 +5210,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B123" s="0" t="n">
         <v>24</v>
@@ -5137,7 +5224,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B124" s="0" t="n">
         <v>24</v>
@@ -5151,7 +5238,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B125" s="0" t="n">
         <v>24</v>
@@ -5165,7 +5252,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B126" s="0" t="n">
         <f aca="false">SUM(B113:B125)</f>

</xml_diff>